<commit_message>
trying to workaround a few more bugs in msvc10 lambdas. also marked a few more expected failures on sfinae not working for private and protected members on older gcc.
</commit_message>
<xml_diff>
--- a/BUGS.xlsx
+++ b/BUGS.xlsx
@@ -173,9 +173,6 @@
 ../boost/any.hpp:169: error: undefined reference to 'operator delete(void*, unsigned int)'</t>
   </si>
   <si>
-    <t>plus a bunch of failure that all seem related to weak lambda support</t>
-  </si>
-  <si>
     <t>hand-full of link errors missing .o files… seems a build server issue on Oct 3-5 (wait an see if it happens in next run)</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>plus a bunch of failure that all seem related to weak lambda support… fixed most of them, plus market lambda in tpl ctor as expected failure</t>
+  </si>
 </sst>
 </file>
 
@@ -422,7 +422,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +461,12 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -493,7 +499,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -584,6 +590,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -871,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +910,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -906,16 +924,16 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>15</v>
@@ -931,29 +949,29 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -964,13 +982,13 @@
     </row>
     <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>42</v>
@@ -982,13 +1000,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>31</v>
@@ -1002,7 +1020,7 @@
     </row>
     <row r="9" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>40</v>
@@ -1014,16 +1032,16 @@
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="12" t="s">
@@ -1037,13 +1055,13 @@
     </row>
     <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>41</v>
@@ -1052,7 +1070,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1062,22 +1080,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>14</v>
@@ -1089,7 +1107,7 @@
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>28</v>
@@ -1103,15 +1121,15 @@
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="33" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -1123,13 +1141,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>23</v>
@@ -1143,13 +1161,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>31</v>
@@ -1172,15 +1190,15 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="32" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -1190,23 +1208,23 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>45</v>
+      <c r="D22" s="34" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1216,28 +1234,28 @@
     </row>
     <row r="25" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="24" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="26" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>1</v>
@@ -1250,7 +1268,7 @@
     </row>
     <row r="27" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
added bjam config requirements on c++11 lambdas, etc. also added a few more expected failures markups
</commit_message>
<xml_diff>
--- a/BUGS.xlsx
+++ b/BUGS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>clang- gnu- linux- 4.0~gnu++11</t>
   </si>
@@ -343,6 +343,11 @@
   <si>
     <t>plus a bunch of failure that all seem related to weak lambda support… fixed most of them, plus market lambda in tpl ctor as expected failure</t>
   </si>
+  <si>
+    <t>comp
+only happens w/ libbc++, it does not happen on same compiler with libstdc++
+it is possible that -lc++api will make this work on libc++ also but not sure…</t>
+  </si>
 </sst>
 </file>
 
@@ -499,7 +504,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -570,6 +575,18 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -591,17 +608,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -889,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,13 +959,13 @@
       <c r="A4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="25" t="s">
         <v>35</v>
       </c>
     </row>
@@ -965,13 +973,13 @@
       <c r="A5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="25" t="s">
         <v>35</v>
       </c>
     </row>
@@ -998,37 +1006,37 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>17</v>
+      <c r="E8" s="35" t="s">
+        <v>59</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="25"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1088,7 +1096,7 @@
       <c r="C14" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="25" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1123,13 +1131,13 @@
       <c r="A17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="26" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -1198,7 +1206,7 @@
       <c r="C21" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="25" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -1210,7 +1218,7 @@
       <c r="C22" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="27" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1218,13 +1226,13 @@
       <c r="A23" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="25" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1239,17 +1247,17 @@
       <c r="B25" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="24" t="s">
+      <c r="E25" s="34"/>
+      <c r="F25" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="28" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1260,11 +1268,11 @@
       <c r="B26" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
@@ -1273,11 +1281,11 @@
       <c r="B27" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>

</xml_diff>